<commit_message>
update wraptext excel phieumuon
fix wraptext
</commit_message>
<xml_diff>
--- a/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/PhieuMuon.xlsx
+++ b/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/PhieuMuon.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODE\DoAnTotNghiep\HUFILibrary\QuanLyThuVienHUFI\Form_QuanLyThuVien\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\DATN\HUFILibrary\QuanLyThuVienHUFI\Form_QuanLyThuVien\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43E468C-E169-4E80-9BBB-63017DB9860D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,9 +179,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -198,7 +194,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -206,6 +201,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -220,6 +218,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,11 +501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,41 +518,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -580,20 +581,20 @@
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -604,44 +605,44 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="9"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="11"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="3:5" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="11"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E20" s="10"/>
+      <c r="E20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>